<commit_message>
nice'n'clean ... finished:pardiso,metis,dmumps,blas&lapack; next:hypre
</commit_message>
<xml_diff>
--- a/checkliste.xlsx
+++ b/checkliste.xlsx
@@ -4,10 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="DevStage" sheetId="1" r:id="rId1"/>
+    <sheet name="Pardiso" sheetId="3" r:id="rId1"/>
+    <sheet name="MUMPS" sheetId="1" r:id="rId2"/>
+    <sheet name="Metis" sheetId="5" r:id="rId3"/>
+    <sheet name="LAPACK+BLAS" sheetId="7" r:id="rId4"/>
+    <sheet name="HYPRE" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="29">
   <si>
     <t>seq</t>
   </si>
@@ -79,6 +83,33 @@
   </si>
   <si>
     <t>no msmpi conflict, versions: msmpi.dll in BoSSS 5.0.124.35.6, mpiexec 4.2.4400.0</t>
+  </si>
+  <si>
+    <t>compiled</t>
+  </si>
+  <si>
+    <t>successful</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>not done yet</t>
+  </si>
+  <si>
+    <t>very large dll: 100 MB</t>
+  </si>
+  <si>
+    <t>mesh quality tested: same partition with old and new metis.dll</t>
+  </si>
+  <si>
+    <t>smaller DLL: 26 mb --&gt; 14 mb</t>
+  </si>
+  <si>
+    <t>OpenMP has weak influence on performance</t>
+  </si>
+  <si>
+    <t>HYPRE</t>
   </si>
 </sst>
 </file>
@@ -120,7 +151,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -128,15 +159,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,7 +534,182 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:E4" si="0">SUM(C10:C15)</f>
+        <f t="shared" ref="C4:D4" si="0">SUM(C10:C15)</f>
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>SUM(E10:E15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <f>SUM(B10:B15)</f>
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:D4" si="0">SUM(C10:C15)</f>
         <v>5</v>
       </c>
       <c r="D4">
@@ -632,6 +881,503 @@
       <c r="F16" t="s">
         <v>19</v>
       </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <f>SUM(B10:B15)</f>
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:D4" si="0">SUM(C10:C15)</f>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>SUM(E10:E15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:F16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <f>SUM(B10:B15)</f>
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:D4" si="0">SUM(C10:C15)</f>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>SUM(E10:E15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <f>SUM(B10:B15)</f>
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:D4" si="0">SUM(C10:C15)</f>
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>SUM(E10:E15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
hopefully everything works now ... next: JENKINS testing
</commit_message>
<xml_diff>
--- a/checkliste.xlsx
+++ b/checkliste.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Pardiso" sheetId="3" r:id="rId1"/>
@@ -1090,7 +1090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -1248,8 +1248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1294,7 +1294,7 @@
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E4">
         <f>SUM(E10:E15)</f>
@@ -1338,15 +1338,24 @@
       <c r="A10" t="s">
         <v>20</v>
       </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>